<commit_message>
Modified evaluation form & some minor documentation refactors
</commit_message>
<xml_diff>
--- a/CG_Homework1_webgl_evaluationform.xlsx
+++ b/CG_Homework1_webgl_evaluationform.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\School\CG_2021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECABA9BD-5C8B-425F-AA2D-C8C1EEAD597A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ACBF87B-BFF8-4518-9C0D-0F7ABDEED522}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Evaluation form" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="51">
   <si>
     <t>Knock-out criteria</t>
   </si>
@@ -148,9 +147,6 @@
     <t>Amount of primitives (10 points)</t>
   </si>
   <si>
-    <t>Floor model, tribune model, road model, wall model, tree model</t>
-  </si>
-  <si>
     <t>s1129160</t>
   </si>
   <si>
@@ -160,9 +156,6 @@
     <t>Gerjan Dijkhuis</t>
   </si>
   <si>
-    <t>Circle geometry, box geometry, cylinder geometry, sphere geometry, torus geometry, custom angle geometry</t>
-  </si>
-  <si>
     <t>We have a skybox.</t>
   </si>
   <si>
@@ -175,10 +168,22 @@
     <t>Usage of the module pattern from the webdev semester, split each 'model' into its own module. Structure makes sense, and naming is clear.</t>
   </si>
   <si>
-    <t xml:space="preserve">We think that a racing track with a moving car is pretty cool. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Applied: material.side, material.color, </t>
+    <t>The car is animated</t>
+  </si>
+  <si>
+    <t>Models imported: Eltjo (as the race car driver), the car and the lights.</t>
+  </si>
+  <si>
+    <t>The tree has 3 different colors applied, lighter-brown for the tree trunk, darker brown for the tree ground and green for the tree's leafs (see: src/world/environment/tree.js). The floor and road make use of textures (also material properties) which comes down to a total of 5. The final material property is applied for the finish line,  which is a white color for the white blocks.</t>
+  </si>
+  <si>
+    <t>Floor model, tribune model, road model, wall model, tree model, finish-line model, red car model, starting-light model.</t>
+  </si>
+  <si>
+    <t>Circle geometry, box geometry, cylinder geometry, sphere geometry, torus geometry, custom angle geometry, rectangle model</t>
+  </si>
+  <si>
+    <t>We think that a racing track with a moving car is pretty cool. Look in the race car when it isn't moving to see even more coolness :)</t>
   </si>
 </sst>
 </file>
@@ -1030,8 +1035,8 @@
   </sheetPr>
   <dimension ref="B2:J36"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1059,7 +1064,7 @@
         <v>25</v>
       </c>
       <c r="E4" s="32" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F4" s="33"/>
     </row>
@@ -1068,7 +1073,7 @@
         <v>26</v>
       </c>
       <c r="E5" s="19" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F5" s="20"/>
     </row>
@@ -1084,7 +1089,7 @@
         <v>28</v>
       </c>
       <c r="E7" s="30" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F7" s="31"/>
     </row>
@@ -1183,42 +1188,44 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:10" ht="45" x14ac:dyDescent="0.25">
       <c r="C20" s="1" t="s">
         <v>22</v>
       </c>
       <c r="E20" s="4"/>
       <c r="F20" s="8"/>
       <c r="H20" s="17" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="21" spans="2:10" ht="45" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" ht="60" x14ac:dyDescent="0.25">
       <c r="C21" s="1" t="s">
         <v>24</v>
       </c>
       <c r="E21" s="5"/>
       <c r="F21" s="9"/>
       <c r="H21" s="17" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" ht="30" x14ac:dyDescent="0.25">
       <c r="C22" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E22" s="14"/>
       <c r="F22" s="9"/>
-      <c r="H22" s="17"/>
-    </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="H22" s="17" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10" ht="150" x14ac:dyDescent="0.25">
       <c r="C23" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E23" s="5"/>
       <c r="F23" s="9"/>
       <c r="H23" s="17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="24" spans="2:10" ht="30" x14ac:dyDescent="0.25">
@@ -1228,7 +1235,7 @@
       <c r="E24" s="5"/>
       <c r="F24" s="9"/>
       <c r="H24" s="17" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.25">
@@ -1238,7 +1245,7 @@
       <c r="E25" s="5"/>
       <c r="F25" s="9"/>
       <c r="H25" s="17" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.25">
@@ -1247,7 +1254,9 @@
       </c>
       <c r="E26" s="5"/>
       <c r="F26" s="9"/>
-      <c r="H26" s="17"/>
+      <c r="H26" s="17" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="27" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C27" s="1" t="s">
@@ -1256,7 +1265,7 @@
       <c r="E27" s="6"/>
       <c r="F27" s="10"/>
       <c r="H27" s="18" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="28" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1299,7 +1308,7 @@
       <c r="E32" s="4"/>
       <c r="F32" s="8"/>
       <c r="H32" s="17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="J32" s="15" t="s">
         <v>21</v>
@@ -1314,14 +1323,14 @@
       <c r="H33" s="26"/>
       <c r="J33" s="27"/>
     </row>
-    <row r="34" spans="2:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C34" s="1" t="s">
         <v>34</v>
       </c>
       <c r="E34" s="6"/>
       <c r="F34" s="10"/>
       <c r="H34" s="18" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="J34" s="16" t="s">
         <v>20</v>
@@ -1355,20 +1364,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_Flow_SignoffStatus xmlns="e7647ff1-e2f7-42a1-a68c-3c96587cf758" xsi:nil="true"/>
-    <SharedWithUsers xmlns="7178be8b-d0ef-4995-97d9-396f4bad9a56">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1612,28 +1613,26 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_Flow_SignoffStatus xmlns="e7647ff1-e2f7-42a1-a68c-3c96587cf758" xsi:nil="true"/>
+    <SharedWithUsers xmlns="7178be8b-d0ef-4995-97d9-396f4bad9a56">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{704D0896-41A1-4D8E-B2B4-DAF4537F2CEF}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{95702B07-5163-4733-93F0-15C1454EB37E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="e7647ff1-e2f7-42a1-a68c-3c96587cf758"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="7178be8b-d0ef-4995-97d9-396f4bad9a56"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1659,9 +1658,19 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{95702B07-5163-4733-93F0-15C1454EB37E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{704D0896-41A1-4D8E-B2B4-DAF4537F2CEF}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="e7647ff1-e2f7-42a1-a68c-3c96587cf758"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="7178be8b-d0ef-4995-97d9-396f4bad9a56"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Final evaluation form for now. Waiting for answers from Eltjo.
</commit_message>
<xml_diff>
--- a/CG_Homework1_webgl_evaluationform.xlsx
+++ b/CG_Homework1_webgl_evaluationform.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\School\CG_2021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ACBF87B-BFF8-4518-9C0D-0F7ABDEED522}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44EF978A-E9C6-484B-BECD-EEDFB507F69E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="53">
   <si>
     <t>Knock-out criteria</t>
   </si>
@@ -162,28 +162,34 @@
     <t>We have a camera.</t>
   </si>
   <si>
-    <t>We have a texture for the floor, and a texture for the road.</t>
-  </si>
-  <si>
     <t>Usage of the module pattern from the webdev semester, split each 'model' into its own module. Structure makes sense, and naming is clear.</t>
   </si>
   <si>
-    <t>The car is animated</t>
-  </si>
-  <si>
     <t>Models imported: Eltjo (as the race car driver), the car and the lights.</t>
   </si>
   <si>
-    <t>The tree has 3 different colors applied, lighter-brown for the tree trunk, darker brown for the tree ground and green for the tree's leafs (see: src/world/environment/tree.js). The floor and road make use of textures (also material properties) which comes down to a total of 5. The final material property is applied for the finish line,  which is a white color for the white blocks.</t>
-  </si>
-  <si>
     <t>Floor model, tribune model, road model, wall model, tree model, finish-line model, red car model, starting-light model.</t>
   </si>
   <si>
-    <t>Circle geometry, box geometry, cylinder geometry, sphere geometry, torus geometry, custom angle geometry, rectangle model</t>
-  </si>
-  <si>
-    <t>We think that a racing track with a moving car is pretty cool. Look in the race car when it isn't moving to see even more coolness :)</t>
+    <t>Circle geometry, box geometry, cylinder geometry, sphere geometry, torus geometry, custom angle geometry, shape geometry</t>
+  </si>
+  <si>
+    <t>The tree has 3 different colors applied, lighter-brown for the tree trunk, darker brown for the tree ground and green for the tree's leafs (see: src/world/environment/tree.js). The floor and road make use of textures (also material properties) which comes down to a total of 5. The final material property is applied for the finish line,  which is a white color for the white blocks. Total material properties: 6.</t>
+  </si>
+  <si>
+    <t>We have a texture for the floor, and a texture for the road. (skybox kind of counts)</t>
+  </si>
+  <si>
+    <t>The car is animated (movement, and wheels), and the lights (light goes from red to green)</t>
+  </si>
+  <si>
+    <t>lots of trees :)</t>
+  </si>
+  <si>
+    <t>We think that a racing track with a moving car is pretty cool. Look in the race car when it isn't moving to see even more coolness :). What is also cool: The light of the sun is aligned with the sun of the skybox. The car's driver (Eltjo) also respects the traffic laws(stops at red light, continues at green light)!</t>
+  </si>
+  <si>
+    <t>s1127251</t>
   </si>
 </sst>
 </file>
@@ -1035,8 +1041,8 @@
   </sheetPr>
   <dimension ref="B2:J36"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A26" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1077,11 +1083,13 @@
       </c>
       <c r="F5" s="20"/>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="C6" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E6" s="19"/>
+      <c r="E6" s="19" t="s">
+        <v>52</v>
+      </c>
       <c r="F6" s="20"/>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
@@ -1195,7 +1203,7 @@
       <c r="E20" s="4"/>
       <c r="F20" s="8"/>
       <c r="H20" s="17" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="21" spans="2:10" ht="60" x14ac:dyDescent="0.25">
@@ -1205,7 +1213,7 @@
       <c r="E21" s="5"/>
       <c r="F21" s="9"/>
       <c r="H21" s="17" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="22" spans="2:10" ht="30" x14ac:dyDescent="0.25">
@@ -1215,10 +1223,10 @@
       <c r="E22" s="14"/>
       <c r="F22" s="9"/>
       <c r="H22" s="17" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="23" spans="2:10" ht="150" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10" ht="165" x14ac:dyDescent="0.25">
       <c r="C23" s="1" t="s">
         <v>11</v>
       </c>
@@ -1228,14 +1236,14 @@
         <v>47</v>
       </c>
     </row>
-    <row r="24" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:10" ht="45" x14ac:dyDescent="0.25">
       <c r="C24" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E24" s="5"/>
       <c r="F24" s="9"/>
       <c r="H24" s="17" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.25">
@@ -1248,14 +1256,14 @@
         <v>41</v>
       </c>
     </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:10" ht="45" x14ac:dyDescent="0.25">
       <c r="C26" s="1" t="s">
         <v>18</v>
       </c>
       <c r="E26" s="5"/>
       <c r="F26" s="9"/>
       <c r="H26" s="17" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
     </row>
     <row r="27" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1308,7 +1316,7 @@
       <c r="E32" s="4"/>
       <c r="F32" s="8"/>
       <c r="H32" s="17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J32" s="15" t="s">
         <v>21</v>
@@ -1320,17 +1328,19 @@
       </c>
       <c r="E33" s="24"/>
       <c r="F33" s="25"/>
-      <c r="H33" s="26"/>
+      <c r="H33" s="26" t="s">
+        <v>50</v>
+      </c>
       <c r="J33" s="27"/>
     </row>
-    <row r="34" spans="2:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:10" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C34" s="1" t="s">
         <v>34</v>
       </c>
       <c r="E34" s="6"/>
       <c r="F34" s="10"/>
       <c r="H34" s="18" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="J34" s="16" t="s">
         <v>20</v>
@@ -1364,12 +1374,20 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_Flow_SignoffStatus xmlns="e7647ff1-e2f7-42a1-a68c-3c96587cf758" xsi:nil="true"/>
+    <SharedWithUsers xmlns="7178be8b-d0ef-4995-97d9-396f4bad9a56">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1613,26 +1631,28 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_Flow_SignoffStatus xmlns="e7647ff1-e2f7-42a1-a68c-3c96587cf758" xsi:nil="true"/>
-    <SharedWithUsers xmlns="7178be8b-d0ef-4995-97d9-396f4bad9a56">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{95702B07-5163-4733-93F0-15C1454EB37E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{704D0896-41A1-4D8E-B2B4-DAF4537F2CEF}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="e7647ff1-e2f7-42a1-a68c-3c96587cf758"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="7178be8b-d0ef-4995-97d9-396f4bad9a56"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1658,19 +1678,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{704D0896-41A1-4D8E-B2B4-DAF4537F2CEF}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{95702B07-5163-4733-93F0-15C1454EB37E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="e7647ff1-e2f7-42a1-a68c-3c96587cf758"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="7178be8b-d0ef-4995-97d9-396f4bad9a56"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>